<commit_message>
Update Subscribe Event Service Specs
Update Subscribe Event Service Specs
</commit_message>
<xml_diff>
--- a/Interface Design.xlsx
+++ b/Interface Design.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26408"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandyturlapaty/Documents/MyComputer/codebase/unfsc-codebase/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Service Name</t>
   </si>
@@ -174,6 +169,24 @@
 "role" : "SystemAnalyst"
 }
 </t>
+  </si>
+  <si>
+    <t>Subscribe Event</t>
+  </si>
+  <si>
+    <t>&lt;application-context&gt;/studentcenter/subscribe-event</t>
+  </si>
+  <si>
+    <t>Content-Type: application/json</t>
+  </si>
+  <si>
+    <t>{
+ "eventId": "14",
+ "userId": "N01"
+}</t>
+  </si>
+  <si>
+    <t>Both are mandatory</t>
   </si>
 </sst>
 </file>
@@ -238,13 +251,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,22 +563,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.1640625" customWidth="1"/>
-    <col min="5" max="5" width="82.33203125" customWidth="1"/>
-    <col min="6" max="6" width="48.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.140625" customWidth="1"/>
+    <col min="5" max="5" width="82.28515625" customWidth="1"/>
+    <col min="6" max="6" width="48.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -584,7 +598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -604,7 +618,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -622,7 +636,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="105" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -642,7 +656,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="300" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="300" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -662,7 +676,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="120" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -682,7 +696,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -700,7 +714,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="180" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -717,6 +731,26 @@
         <v>30</v>
       </c>
       <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>